<commit_message>
Entity, DTO, Repisitory Unify
</commit_message>
<xml_diff>
--- a/database/ER.xlsx
+++ b/database/ER.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\DACNPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\DACNPM\DACN-2022\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA6A13-B7F0-45DB-A4FA-FDA770E87093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A58B3CA-C073-49D3-AC7F-0056FA1BDE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{88D34EA1-CE92-4B3E-BB8F-076EA833F96D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="80">
   <si>
     <t>id</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>CommentQuote: 200</t>
+  </si>
+  <si>
+    <t>nvarchar(2000)</t>
+  </si>
+  <si>
+    <t>varchar(2000)</t>
+  </si>
+  <si>
+    <t>varchar(1000)</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
 </sst>
 </file>
@@ -476,6 +488,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,21 +501,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -509,9 +512,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -519,6 +519,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,6 +540,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -858,47 +870,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23C9432-A9AF-4EC8-86C8-00C10D60561F}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54:O54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="35" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="E1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="33" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="I1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="M1" s="36" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="M1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -919,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -928,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>4</v>
@@ -937,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>4</v>
@@ -946,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>4</v>
@@ -1036,11 +1048,11 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1078,18 +1090,18 @@
       <c r="K8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -1105,9 +1117,11 @@
         <v>22</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
@@ -1117,7 +1131,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1133,14 +1147,14 @@
         <v>23</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K10" s="7"/>
       <c r="M10" s="14" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>4</v>
@@ -1151,7 +1165,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
@@ -1176,7 +1190,7 @@
         <v>30</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O11" s="14" t="s">
         <v>4</v>
@@ -1196,7 +1210,7 @@
         <v>18</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O12" s="14" t="s">
         <v>4</v>
@@ -1216,28 +1230,28 @@
         <v>51</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O13" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="E14" s="26" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="E14" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
       <c r="I14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>4</v>
@@ -1246,7 +1260,7 @@
         <v>63</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O14" s="14" t="s">
         <v>27</v>
@@ -1263,7 +1277,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>27</v>
@@ -1274,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1283,23 +1297,23 @@
         <v>0</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1316,18 +1330,18 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="M17" s="31" t="s">
+      <c r="M17" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>57</v>
@@ -1336,14 +1350,14 @@
         <v>34</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="G18" s="5"/>
       <c r="I18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>4</v>
@@ -1375,7 +1389,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>4</v>
@@ -1384,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>4</v>
@@ -1395,9 +1409,11 @@
         <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
@@ -1409,7 +1425,7 @@
         <v>38</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>4</v>
@@ -1418,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>4</v>
@@ -1429,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C21" s="4"/>
       <c r="E21" s="5" t="s">
@@ -1443,7 +1459,7 @@
         <v>28</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>4</v>
@@ -1481,31 +1497,33 @@
         <v>22</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="I23" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G24" s="5"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-      <c r="M24" s="32" t="s">
+      <c r="M24" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E25" s="5" t="s">
@@ -1519,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>4</v>
@@ -1529,11 +1547,11 @@
       <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
       <c r="E26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1547,7 +1565,7 @@
         <v>2</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>4</v>
@@ -1556,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O26" s="16" t="s">
         <v>4</v>
@@ -1579,7 +1597,7 @@
         <v>21</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K27" s="10" t="s">
         <v>43</v>
@@ -1599,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>4</v>
@@ -1608,7 +1626,7 @@
         <v>33</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>4</v>
@@ -1626,7 +1644,7 @@
         <v>44</v>
       </c>
       <c r="N28" s="16" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="O28" s="16" t="s">
         <v>4</v>
@@ -1637,7 +1655,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>4</v>
@@ -1646,14 +1664,16 @@
         <v>22</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="M29" s="16" t="s">
         <v>30</v>
       </c>
       <c r="N29" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O29" s="16" t="s">
         <v>4</v>
@@ -1664,7 +1684,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>4</v>
@@ -1673,25 +1693,25 @@
         <v>23</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K30" s="10"/>
       <c r="M30" s="16" t="s">
         <v>18</v>
       </c>
       <c r="N30" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O30" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
       <c r="I31" s="10" t="s">
         <v>24</v>
       </c>
@@ -1724,16 +1744,16 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
       <c r="E33" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>4</v>
@@ -1752,23 +1772,23 @@
       <c r="G34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="J34" s="29"/>
-      <c r="K34" s="30"/>
-      <c r="M34" s="32" t="s">
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+      <c r="M34" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>4</v>
@@ -1777,7 +1797,7 @@
         <v>35</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>4</v>
@@ -1794,7 +1814,7 @@
         <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>4</v>
@@ -1812,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K36" s="11" t="s">
         <v>4</v>
@@ -1821,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O36" s="16" t="s">
         <v>4</v>
@@ -1832,7 +1852,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>4</v>
@@ -1841,7 +1861,7 @@
         <v>30</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>4</v>
@@ -1879,7 +1899,7 @@
         <v>44</v>
       </c>
       <c r="N38" s="16" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="O38" s="16" t="s">
         <v>4</v>
@@ -1890,42 +1910,42 @@
         <v>34</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="K39" s="11"/>
       <c r="M39" s="16" t="s">
         <v>39</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O39" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="E40" s="20" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="E40" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
       <c r="I40" s="11" t="s">
         <v>38</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K40" s="11"/>
       <c r="M40" s="16" t="s">
         <v>18</v>
       </c>
       <c r="N40" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O40" s="16" t="s">
         <v>4</v>
@@ -1942,9 +1962,11 @@
         <v>22</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="M41" s="16" t="s">
         <v>45</v>
       </c>
@@ -1960,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>4</v>
@@ -1969,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>4</v>
@@ -1978,7 +2000,7 @@
         <v>23</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="K42" s="11"/>
     </row>
@@ -1987,7 +2009,7 @@
         <v>18</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>4</v>
@@ -2014,7 +2036,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>4</v>
@@ -2037,11 +2059,11 @@
       <c r="K44" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M44" s="23" t="s">
+      <c r="M44" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E45" s="8" t="s">
@@ -2071,7 +2093,7 @@
         <v>30</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>4</v>
@@ -2080,7 +2102,7 @@
         <v>33</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K46" s="11" t="s">
         <v>4</v>
@@ -2089,9 +2111,11 @@
         <v>0</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O46" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M47" s="1" t="s">
@@ -2100,30 +2124,36 @@
       <c r="N47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O47" s="1"/>
+      <c r="O47" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O48" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
       <c r="M49" s="19" t="s">
         <v>21</v>
       </c>
       <c r="N49" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O49" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="50" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E50" s="8"/>
@@ -2133,16 +2163,18 @@
         <v>18</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O50" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E51" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>4</v>
@@ -2153,7 +2185,9 @@
       <c r="N51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O51" s="1"/>
+      <c r="O51" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E52" s="8" t="s">
@@ -2171,7 +2205,7 @@
         <v>35</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>4</v>
@@ -2187,18 +2221,18 @@
       <c r="G54" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M54" s="23" t="s">
+      <c r="M54" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="N54" s="23"/>
-      <c r="O54" s="23"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
     </row>
     <row r="55" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E55" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>4</v>
@@ -2212,9 +2246,11 @@
         <v>0</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O56" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M57" s="1" t="s">
@@ -2223,34 +2259,42 @@
       <c r="N57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O57" s="1"/>
+      <c r="O57" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M58" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O58" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M59" s="19" t="s">
         <v>21</v>
       </c>
       <c r="N59" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O59" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="60" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O60" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="61" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M61" s="1" t="s">
@@ -2259,16 +2303,12 @@
       <c r="N61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O61" s="1"/>
+      <c r="O61" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="M17:O17"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M34:O34"/>
     <mergeCell ref="I1:K1"/>
@@ -2277,6 +2317,12 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="M17:O17"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="E49:G49"/>

</xml_diff>

<commit_message>
Unify DTO, Entity, Repository
</commit_message>
<xml_diff>
--- a/database/ER.xlsx
+++ b/database/ER.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\DACNPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\DACNPM\DACN-2022\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA6A13-B7F0-45DB-A4FA-FDA770E87093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A58B3CA-C073-49D3-AC7F-0056FA1BDE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{88D34EA1-CE92-4B3E-BB8F-076EA833F96D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="80">
   <si>
     <t>id</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>CommentQuote: 200</t>
+  </si>
+  <si>
+    <t>nvarchar(2000)</t>
+  </si>
+  <si>
+    <t>varchar(2000)</t>
+  </si>
+  <si>
+    <t>varchar(1000)</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
 </sst>
 </file>
@@ -476,6 +488,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,21 +501,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -509,9 +512,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -519,6 +519,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,6 +540,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -858,47 +870,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23C9432-A9AF-4EC8-86C8-00C10D60561F}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54:O54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="35" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="E1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="33" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="I1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="M1" s="36" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="M1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -919,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -928,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>4</v>
@@ -937,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>4</v>
@@ -946,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>4</v>
@@ -1036,11 +1048,11 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1078,18 +1090,18 @@
       <c r="K8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -1105,9 +1117,11 @@
         <v>22</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
@@ -1117,7 +1131,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1133,14 +1147,14 @@
         <v>23</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K10" s="7"/>
       <c r="M10" s="14" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>4</v>
@@ -1151,7 +1165,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
@@ -1176,7 +1190,7 @@
         <v>30</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O11" s="14" t="s">
         <v>4</v>
@@ -1196,7 +1210,7 @@
         <v>18</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O12" s="14" t="s">
         <v>4</v>
@@ -1216,28 +1230,28 @@
         <v>51</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O13" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="E14" s="26" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="E14" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
       <c r="I14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>4</v>
@@ -1246,7 +1260,7 @@
         <v>63</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O14" s="14" t="s">
         <v>27</v>
@@ -1263,7 +1277,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>27</v>
@@ -1274,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1283,23 +1297,23 @@
         <v>0</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1316,18 +1330,18 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="M17" s="31" t="s">
+      <c r="M17" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>57</v>
@@ -1336,14 +1350,14 @@
         <v>34</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="G18" s="5"/>
       <c r="I18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>4</v>
@@ -1375,7 +1389,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>4</v>
@@ -1384,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>4</v>
@@ -1395,9 +1409,11 @@
         <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
@@ -1409,7 +1425,7 @@
         <v>38</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>4</v>
@@ -1418,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>4</v>
@@ -1429,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C21" s="4"/>
       <c r="E21" s="5" t="s">
@@ -1443,7 +1459,7 @@
         <v>28</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>4</v>
@@ -1481,31 +1497,33 @@
         <v>22</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="I23" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G24" s="5"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-      <c r="M24" s="32" t="s">
+      <c r="M24" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E25" s="5" t="s">
@@ -1519,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>4</v>
@@ -1529,11 +1547,11 @@
       <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
       <c r="E26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1547,7 +1565,7 @@
         <v>2</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>4</v>
@@ -1556,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O26" s="16" t="s">
         <v>4</v>
@@ -1579,7 +1597,7 @@
         <v>21</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K27" s="10" t="s">
         <v>43</v>
@@ -1599,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>4</v>
@@ -1608,7 +1626,7 @@
         <v>33</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>4</v>
@@ -1626,7 +1644,7 @@
         <v>44</v>
       </c>
       <c r="N28" s="16" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="O28" s="16" t="s">
         <v>4</v>
@@ -1637,7 +1655,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>4</v>
@@ -1646,14 +1664,16 @@
         <v>22</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="M29" s="16" t="s">
         <v>30</v>
       </c>
       <c r="N29" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O29" s="16" t="s">
         <v>4</v>
@@ -1664,7 +1684,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>4</v>
@@ -1673,25 +1693,25 @@
         <v>23</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K30" s="10"/>
       <c r="M30" s="16" t="s">
         <v>18</v>
       </c>
       <c r="N30" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O30" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
       <c r="I31" s="10" t="s">
         <v>24</v>
       </c>
@@ -1724,16 +1744,16 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
       <c r="E33" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>4</v>
@@ -1752,23 +1772,23 @@
       <c r="G34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="J34" s="29"/>
-      <c r="K34" s="30"/>
-      <c r="M34" s="32" t="s">
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+      <c r="M34" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>4</v>
@@ -1777,7 +1797,7 @@
         <v>35</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>4</v>
@@ -1794,7 +1814,7 @@
         <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>4</v>
@@ -1812,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K36" s="11" t="s">
         <v>4</v>
@@ -1821,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O36" s="16" t="s">
         <v>4</v>
@@ -1832,7 +1852,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>4</v>
@@ -1841,7 +1861,7 @@
         <v>30</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>4</v>
@@ -1879,7 +1899,7 @@
         <v>44</v>
       </c>
       <c r="N38" s="16" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="O38" s="16" t="s">
         <v>4</v>
@@ -1890,42 +1910,42 @@
         <v>34</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="K39" s="11"/>
       <c r="M39" s="16" t="s">
         <v>39</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O39" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="E40" s="20" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="E40" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
       <c r="I40" s="11" t="s">
         <v>38</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K40" s="11"/>
       <c r="M40" s="16" t="s">
         <v>18</v>
       </c>
       <c r="N40" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O40" s="16" t="s">
         <v>4</v>
@@ -1942,9 +1962,11 @@
         <v>22</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="M41" s="16" t="s">
         <v>45</v>
       </c>
@@ -1960,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>4</v>
@@ -1969,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>4</v>
@@ -1978,7 +2000,7 @@
         <v>23</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="K42" s="11"/>
     </row>
@@ -1987,7 +2009,7 @@
         <v>18</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>4</v>
@@ -2014,7 +2036,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>4</v>
@@ -2037,11 +2059,11 @@
       <c r="K44" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M44" s="23" t="s">
+      <c r="M44" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E45" s="8" t="s">
@@ -2071,7 +2093,7 @@
         <v>30</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>4</v>
@@ -2080,7 +2102,7 @@
         <v>33</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="K46" s="11" t="s">
         <v>4</v>
@@ -2089,9 +2111,11 @@
         <v>0</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O46" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M47" s="1" t="s">
@@ -2100,30 +2124,36 @@
       <c r="N47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O47" s="1"/>
+      <c r="O47" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O48" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
       <c r="M49" s="19" t="s">
         <v>21</v>
       </c>
       <c r="N49" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O49" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="50" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E50" s="8"/>
@@ -2133,16 +2163,18 @@
         <v>18</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O50" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E51" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>4</v>
@@ -2153,7 +2185,9 @@
       <c r="N51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O51" s="1"/>
+      <c r="O51" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E52" s="8" t="s">
@@ -2171,7 +2205,7 @@
         <v>35</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>4</v>
@@ -2187,18 +2221,18 @@
       <c r="G54" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M54" s="23" t="s">
+      <c r="M54" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="N54" s="23"/>
-      <c r="O54" s="23"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
     </row>
     <row r="55" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E55" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>4</v>
@@ -2212,9 +2246,11 @@
         <v>0</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O56" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M57" s="1" t="s">
@@ -2223,34 +2259,42 @@
       <c r="N57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O57" s="1"/>
+      <c r="O57" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M58" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O58" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M59" s="19" t="s">
         <v>21</v>
       </c>
       <c r="N59" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O59" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="60" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O60" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="61" spans="5:15" x14ac:dyDescent="0.2">
       <c r="M61" s="1" t="s">
@@ -2259,16 +2303,12 @@
       <c r="N61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O61" s="1"/>
+      <c r="O61" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="M17:O17"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M34:O34"/>
     <mergeCell ref="I1:K1"/>
@@ -2277,6 +2317,12 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="M17:O17"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="E49:G49"/>

</xml_diff>